<commit_message>
how to choose or use design pattern
</commit_message>
<xml_diff>
--- a/design-pattern/内容出处.xlsx
+++ b/design-pattern/内容出处.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11">
   <si>
     <t>设计模式分类及概述总览.xlsx</t>
   </si>
@@ -27,16 +27,37 @@
   <si>
     <t>《设计模式-可复用面向对象软件的基础》-1.5</t>
   </si>
+  <si>
+    <t>如何使用设计模式.txt</t>
+  </si>
+  <si>
+    <t>《设计模式-可复用面向对象软件的基础》-1.8</t>
+  </si>
+  <si>
+    <t>如何选择设计模式.txt</t>
+  </si>
+  <si>
+    <t>《设计模式-可复用面向对象软件的基础》-1.7</t>
+  </si>
+  <si>
+    <t>设计模式不能随意使用.txt</t>
+  </si>
+  <si>
+    <t>《设计模式-可复用面向对象软件的基础》-P21 第一章结尾</t>
+  </si>
+  <si>
+    <t>设计模式所支持的设计的可变方面.xlsx</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -54,11 +75,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -70,28 +97,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -108,9 +113,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -118,39 +130,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -162,30 +144,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,31 +221,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -236,13 +323,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -254,133 +389,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,7 +428,22 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -416,7 +452,33 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
         <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -450,191 +512,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -964,13 +985,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="31.2142857142857" customWidth="1"/>
     <col min="2" max="2" width="53.0714285714286" customWidth="1"/>
@@ -992,6 +1013,38 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>

</xml_diff>